<commit_message>
completo las 100 direcciones para comparar
</commit_message>
<xml_diff>
--- a/direccionesVerificadas.xlsx
+++ b/direccionesVerificadas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="552">
   <si>
     <t xml:space="preserve">direccion</t>
   </si>
@@ -34,13 +34,10 @@
     <t xml:space="preserve">longitud</t>
   </si>
   <si>
-    <t xml:space="preserve">latitud verificada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitud verificada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distancia</t>
+    <t xml:space="preserve">latitud_verificada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitud_verificada</t>
   </si>
   <si>
     <t xml:space="preserve">MANUEL CORVALAN 1700, Avellaneda, Buenos Aires</t>
@@ -97,16 +94,19 @@
     <t xml:space="preserve">-57.966953262027154</t>
   </si>
   <si>
-    <t xml:space="preserve">CALLE 80 (ESQUINA CALLE 159), La Plata, Buenos Aires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-34.9869863020363</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-57.9726516121067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no encuentra</t>
+    <t xml:space="preserve">AVENIDA 1 (ENTRE AVENIDA 44 Y CALLE 45), La Plata, Buenos Aires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-34.90548231099285</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.948549247098995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-34.90548338867588</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.948413876079236</t>
   </si>
   <si>
     <t xml:space="preserve">SUIPACHA 3571, Lanús, Buenos Aires</t>
@@ -226,25 +226,37 @@
     <t xml:space="preserve">-56.712012775432626</t>
   </si>
   <si>
-    <t xml:space="preserve">C 536 - JUNCAL 68, Necochea, Buenos Aires</t>
+    <t xml:space="preserve">C 89 - TGRL PABLO RICHIERI (ESQUINA C 64 - BALCARCE), Necochea, Buenos Aires</t>
   </si>
   <si>
     <t xml:space="preserve">Necochea - Quequen</t>
   </si>
   <si>
-    <t xml:space="preserve">-38.57080092526957</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-58.71307028888971</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C 570 - PASO 181, Necochea, Buenos Aires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-38.55263536830426</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-58.723083035022974</t>
+    <t xml:space="preserve">-38.5636975446619</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.7565589135345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-38.563614081307044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.75659483299326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AV 10 - RCA ORIENTAL DEL URUGUAY 200, Necochea, Buenos Aires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-38.59554675212798</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.77757920872384</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-38.60526678319084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.80430530415515</t>
   </si>
   <si>
     <t xml:space="preserve">ELISEO RECLUS 852, San Isidro, Buenos Aires</t>
@@ -328,6 +340,12 @@
     <t xml:space="preserve">-57.99427212331911</t>
   </si>
   <si>
+    <t xml:space="preserve">-35.58175977754936</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.99430243445999</t>
+  </si>
+  <si>
     <t xml:space="preserve">AV HIPOLITO YRIGOYEN (ESQUINA AV LASTRA), Chascomús, Buenos Aires</t>
   </si>
   <si>
@@ -337,6 +355,12 @@
     <t xml:space="preserve">-58.0082209684804</t>
   </si>
   <si>
+    <t xml:space="preserve">-35.57706680716753</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.00892628071439</t>
+  </si>
+  <si>
     <t xml:space="preserve">JUAN B JUSTO 1700, Merlo, Buenos Aires</t>
   </si>
   <si>
@@ -349,6 +373,12 @@
     <t xml:space="preserve">-58.7014640398186</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.68631123625656</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.702375124735326</t>
+  </si>
+  <si>
     <t xml:space="preserve">MENDOZA 600, Merlo, Buenos Aires</t>
   </si>
   <si>
@@ -358,6 +388,12 @@
     <t xml:space="preserve">-58.7336462874051</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.66990983905484</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.73375251971078</t>
+  </si>
+  <si>
     <t xml:space="preserve">CNL BRANDSEN 5300, Avellaneda, Buenos Aires</t>
   </si>
   <si>
@@ -367,6 +403,12 @@
     <t xml:space="preserve">-58.3285801785781</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.69763849382144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.32805700436667</t>
+  </si>
+  <si>
     <t xml:space="preserve">GRL LEMOS 31, Avellaneda, Buenos Aires</t>
   </si>
   <si>
@@ -376,6 +418,12 @@
     <t xml:space="preserve">-58.35429070272847</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.67088093546317</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.35429373320383</t>
+  </si>
+  <si>
     <t xml:space="preserve">OLD MAN (ESQUINA MANANTIAL), Escobar, Buenos Aires</t>
   </si>
   <si>
@@ -388,6 +436,12 @@
     <t xml:space="preserve">-58.8485840993179</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.34239222148232</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.84859316205636</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALLE RAWSON 300, Escobar, Buenos Aires</t>
   </si>
   <si>
@@ -397,6 +451,12 @@
     <t xml:space="preserve">-58.72747734388601</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.353547958209674</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.7864645620557</t>
+  </si>
+  <si>
     <t xml:space="preserve">ISABEL CEBEY, Tigre, Buenos Aires</t>
   </si>
   <si>
@@ -406,13 +466,25 @@
     <t xml:space="preserve">-58.6292984996351</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.465324697024826</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.63034583614817</t>
+  </si>
+  <si>
     <t xml:space="preserve">SARGENTO CABRAL, Tigre, Buenos Aires</t>
   </si>
   <si>
-    <t xml:space="preserve">-34.4424399729544</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-58.58287909298255</t>
+    <t xml:space="preserve">-34.491833292424765</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.62058043338897</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-34.49163090222773</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.620408162048626</t>
   </si>
   <si>
     <t xml:space="preserve">CALLE N 125 (ENTRE CALLE N 36 Y CALLE N 37), Ensenada, Buenos Aires</t>
@@ -427,6 +499,12 @@
     <t xml:space="preserve">-57.94576775398585</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.88835607488309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.94577051231372</t>
+  </si>
+  <si>
     <t xml:space="preserve">40 BRASIL (ENTRE 37 BOSSINGA Y INDEPENDENCIA), Ensenada, Buenos Aires</t>
   </si>
   <si>
@@ -436,6 +514,12 @@
     <t xml:space="preserve">-57.91441090526445</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.85836998794177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.91430478739829</t>
+  </si>
+  <si>
     <t xml:space="preserve">MARCOS SASTRE 2500, Tigre, Buenos Aires</t>
   </si>
   <si>
@@ -445,6 +529,12 @@
     <t xml:space="preserve">-58.596364599208464</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.41950877125666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.596783324311666</t>
+  </si>
+  <si>
     <t xml:space="preserve">LUIS GARCIA 1014, Tigre, Buenos Aires</t>
   </si>
   <si>
@@ -454,6 +544,12 @@
     <t xml:space="preserve">-58.583634647381714</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.42895217863186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.58366936020227</t>
+  </si>
+  <si>
     <t xml:space="preserve">MAIPU (ESQUINA FRANCISCO CESTINO), Ensenada, Buenos Aires</t>
   </si>
   <si>
@@ -463,6 +559,12 @@
     <t xml:space="preserve">-57.92768716239</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.85597015292944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.92766983319423</t>
+  </si>
+  <si>
     <t xml:space="preserve">GILBERTO GAGGINO (ENTRE CORRIENTES Y SAN LUIS), Ensenada, Buenos Aires</t>
   </si>
   <si>
@@ -472,6 +574,12 @@
     <t xml:space="preserve">-57.89328867956805</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.85383190792044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.89332906909811</t>
+  </si>
+  <si>
     <t xml:space="preserve">EZEQUIEL PEREZ IGLESIAS 600, Esteban Echeverría, Buenos Aires</t>
   </si>
   <si>
@@ -484,6 +592,12 @@
     <t xml:space="preserve">-58.4682363866817</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.802734853519894</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.468263504361374</t>
+  </si>
+  <si>
     <t xml:space="preserve">FERNANDEZ MORENO 50, Esteban Echeverría, Buenos Aires</t>
   </si>
   <si>
@@ -493,6 +607,12 @@
     <t xml:space="preserve">-58.49995107382695</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.82983163895666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.50007981785288</t>
+  </si>
+  <si>
     <t xml:space="preserve">MARONI ENRIQUE P 469, Bragado, Buenos Aires</t>
   </si>
   <si>
@@ -505,6 +625,12 @@
     <t xml:space="preserve">-60.487084613268216</t>
   </si>
   <si>
+    <t xml:space="preserve">-35.12329779306783</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-60.48727397735861</t>
+  </si>
+  <si>
     <t xml:space="preserve">RIVADAVIA 2379, Bragado, Buenos Aires</t>
   </si>
   <si>
@@ -514,6 +640,12 @@
     <t xml:space="preserve">-60.47513677599636</t>
   </si>
   <si>
+    <t xml:space="preserve">-35.121599867228745</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-60.474362477358575</t>
+  </si>
+  <si>
     <t xml:space="preserve">JOSE ZANDALAZINI (ESQUINA CORONEL DORREGO), Ramallo, Buenos Aires</t>
   </si>
   <si>
@@ -526,6 +658,12 @@
     <t xml:space="preserve">-60.0515889371472</t>
   </si>
   <si>
+    <t xml:space="preserve">-33.512828668695576</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-60.05155338355385</t>
+  </si>
+  <si>
     <t xml:space="preserve">YRIGOYEN (ENTRE RO BLANCO Y RAUL ROSSI), Ramallo, Buenos Aires</t>
   </si>
   <si>
@@ -535,6 +673,12 @@
     <t xml:space="preserve">-60.050784014212894</t>
   </si>
   <si>
+    <t xml:space="preserve">-33.490788604779205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-60.050820251786405</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAN LORENZO 1000, Ramallo, Buenos Aires</t>
   </si>
   <si>
@@ -547,6 +691,12 @@
     <t xml:space="preserve">-59.9959540766371</t>
   </si>
   <si>
+    <t xml:space="preserve">-33.480431187500066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-59.99625653173621</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESTEBAN ECHEVERRIA (ENTRE OLEGARIO V ANDRADE Y JOSE INGENIEROS), Mar Chiquita, Buenos Aires</t>
   </si>
   <si>
@@ -559,6 +709,12 @@
     <t xml:space="preserve">-57.428151000651695</t>
   </si>
   <si>
+    <t xml:space="preserve">-37.74174866342025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.42827310437258</t>
+  </si>
+  <si>
     <t xml:space="preserve">COMANDANTE CORDOBA 635, General Pinto, Buenos Aires</t>
   </si>
   <si>
@@ -571,6 +727,12 @@
     <t xml:space="preserve">-61.89457043686376</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.76631325077219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-61.89416567552766</t>
+  </si>
+  <si>
     <t xml:space="preserve">ARTURO CAPDEVILLA (ENTRE GABRIELA MISTRAL Y CONRADO N ROXLO), Mar Chiquita, Buenos Aires</t>
   </si>
   <si>
@@ -580,16 +742,28 @@
     <t xml:space="preserve">-57.43634226768505</t>
   </si>
   <si>
-    <t xml:space="preserve">USPALLATA, Coronel Suárez, Buenos Aires</t>
+    <t xml:space="preserve">-37.74114476895858</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.43639096065569</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USPALLATA (ENTRE SGTO BAIGORRIA Y PLUMERILLO), Coronel Suárez, Buenos Aires</t>
   </si>
   <si>
     <t xml:space="preserve">Coronel Suárez</t>
   </si>
   <si>
-    <t xml:space="preserve">-37.46156613858885</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-61.93940585968195</t>
+    <t xml:space="preserve">-37.4634939683587</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-61.93895482351985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-37.46348105690972</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-61.9390794222782</t>
   </si>
   <si>
     <t xml:space="preserve">BELGRANO 276, Dolores, Buenos Aires</t>
@@ -604,6 +778,12 @@
     <t xml:space="preserve">-57.67610409742886</t>
   </si>
   <si>
+    <t xml:space="preserve">-36.316181351149915</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.67611644067065</t>
+  </si>
+  <si>
     <t xml:space="preserve">BELGRANO 1550, Dolores, Buenos Aires</t>
   </si>
   <si>
@@ -613,6 +793,12 @@
     <t xml:space="preserve">-57.662430064332</t>
   </si>
   <si>
+    <t xml:space="preserve">-36.31070926336253</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.66242640428171</t>
+  </si>
+  <si>
     <t xml:space="preserve">58 SAN MARTIN (ENTRE C 65 - 25 DE MAYO Y 67 9 DE JULIO), Olavarría, Buenos Aires</t>
   </si>
   <si>
@@ -625,16 +811,28 @@
     <t xml:space="preserve">-60.318678410075805</t>
   </si>
   <si>
-    <t xml:space="preserve">CALLE 58 (ESQUINA CALLE 133 DE LAS TROPAS), General Belgrano, Buenos Aires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General Belgrano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-35.7539602603274</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-58.4942315913153</t>
+    <t xml:space="preserve">-36.896844397457244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-60.31872708377202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AV COSTANERA JM DE ROSAS (ESQUINA CALLE 17 FRAY F MARTINEZ), Monte, Buenos Aires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Miguel del Monte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-35.4458822977302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.8066309542302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-35.44576241299979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.80671772762894</t>
   </si>
   <si>
     <t xml:space="preserve">RUTA PCIAL 58-MARIANO CASTEX AV 16, Ezeiza, Buenos Aires</t>
@@ -649,16 +847,25 @@
     <t xml:space="preserve">-58.50286882028849</t>
   </si>
   <si>
-    <t xml:space="preserve">LAS GARZAS, Monte, Buenos Aires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">San Miguel del Monte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-35.44740047320195</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-58.81900982102775</t>
+    <t xml:space="preserve">-34.89778198000933</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.50880045814848</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALLE 12 HIPOLITO YRIGOYEN 64, Monte, Buenos Aires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-35.44100477965121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.79896956797337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-35.44094105295223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.79941259567344</t>
   </si>
   <si>
     <t xml:space="preserve">CASEROS 1200, Ezeiza, Buenos Aires</t>
@@ -670,16 +877,28 @@
     <t xml:space="preserve">-58.50687636319143</t>
   </si>
   <si>
-    <t xml:space="preserve">RUTA PCIAL 36-CALCHAQUI AV 32.5, Florencio Varela, Buenos Aires</t>
+    <t xml:space="preserve">-34.84384316204858</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.51029736203039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">228 TGRL JUAN DOMINGO PERON 800, Florencio Varela, Buenos Aires</t>
   </si>
   <si>
     <t xml:space="preserve">Florencio Varela</t>
   </si>
   <si>
-    <t xml:space="preserve">-34.828597653935205</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-58.21833516833528</t>
+    <t xml:space="preserve">-34.8062982936223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.2499893428245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-34.8062943684584</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.25048717737496</t>
   </si>
   <si>
     <t xml:space="preserve">AV BOSQUES 2700, Florencio Varela, Buenos Aires</t>
@@ -691,6 +910,12 @@
     <t xml:space="preserve">-58.22964504984735</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.80833518208645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.227921748539345</t>
+  </si>
+  <si>
     <t xml:space="preserve">220 SAN JUAN 74, Florencio Varela, Buenos Aires</t>
   </si>
   <si>
@@ -700,6 +925,12 @@
     <t xml:space="preserve">-58.27675002815287</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.806506433792734</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.27702919086817</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANCHORENA 1181, Baradero, Buenos Aires</t>
   </si>
   <si>
@@ -712,6 +943,12 @@
     <t xml:space="preserve">-59.50292775964548</t>
   </si>
   <si>
+    <t xml:space="preserve">-33.80909509600629</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-59.503465353828474</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALLE 34 1090, General Alvarado, Buenos Aires</t>
   </si>
   <si>
@@ -724,6 +961,12 @@
     <t xml:space="preserve">-57.84160334221234</t>
   </si>
   <si>
+    <t xml:space="preserve">-38.26700459495411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.842083533009955</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALLE 22 700, General Alvarado, Buenos Aires</t>
   </si>
   <si>
@@ -733,6 +976,12 @@
     <t xml:space="preserve">-57.8329217784653</t>
   </si>
   <si>
+    <t xml:space="preserve">-38.268197756720866</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.833785433009794</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALLE 55 BUENOS AIRES 5000, General San Martín, Buenos Aires</t>
   </si>
   <si>
@@ -745,6 +994,12 @@
     <t xml:space="preserve">-58.5527427324099</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.54632159897925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.55274326204584</t>
+  </si>
+  <si>
     <t xml:space="preserve">GRL OCAMPO 3200, La Matanza, Buenos Aires</t>
   </si>
   <si>
@@ -757,6 +1012,12 @@
     <t xml:space="preserve">-58.5574635861051</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.67688925892887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.557438611245</t>
+  </si>
+  <si>
     <t xml:space="preserve">AVELLANEDA 700, La Matanza, Buenos Aires</t>
   </si>
   <si>
@@ -766,6 +1027,12 @@
     <t xml:space="preserve">-58.53908720825869</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.64750549917977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.56730779087621</t>
+  </si>
+  <si>
     <t xml:space="preserve">RINCON 400, Lomas de Zamora, Buenos Aires</t>
   </si>
   <si>
@@ -778,6 +1045,12 @@
     <t xml:space="preserve">-58.3896576626143</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.741343575488436</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.389795548542786</t>
+  </si>
+  <si>
     <t xml:space="preserve">JUAN BAUTISTA ALBERDI 1600, Vicente López, Buenos Aires</t>
   </si>
   <si>
@@ -790,6 +1063,12 @@
     <t xml:space="preserve">-58.4922855057213</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.51107365837626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.49223892951279</t>
+  </si>
+  <si>
     <t xml:space="preserve">AV LA AVIACION 1231, Almirante Brown, Buenos Aires</t>
   </si>
   <si>
@@ -802,6 +1081,12 @@
     <t xml:space="preserve">-58.38677134247924</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.86557071381206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.386982735043404</t>
+  </si>
+  <si>
     <t xml:space="preserve">R DE ESCALADA 46, La Matanza, Buenos Aires</t>
   </si>
   <si>
@@ -811,6 +1096,12 @@
     <t xml:space="preserve">-58.55997826878636</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.6388894928246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.56023027738373</t>
+  </si>
+  <si>
     <t xml:space="preserve">24 DE OCTUBRE 641, Ituzaingó, Buenos Aires</t>
   </si>
   <si>
@@ -823,6 +1114,12 @@
     <t xml:space="preserve">-58.66302329900425</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.65946812348925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.663165062040065</t>
+  </si>
+  <si>
     <t xml:space="preserve">CAMACUA (ESQUINA GRL FELIX DE OLAZABAL), Ituzaingó, Buenos Aires</t>
   </si>
   <si>
@@ -832,6 +1129,12 @@
     <t xml:space="preserve">-58.6641946381337</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.65577144614452</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.66419623320452</t>
+  </si>
+  <si>
     <t xml:space="preserve">CONVENCION 1407, La Matanza, Buenos Aires</t>
   </si>
   <si>
@@ -841,6 +1144,12 @@
     <t xml:space="preserve">-58.506814302352126</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.69572621226854</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.50670906706113</t>
+  </si>
+  <si>
     <t xml:space="preserve">COLETTA ANTONIO 829, Campana, Buenos Aires</t>
   </si>
   <si>
@@ -853,6 +1162,12 @@
     <t xml:space="preserve">-58.96024791517884</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.16849237534577</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.96033213838101</t>
+  </si>
+  <si>
     <t xml:space="preserve">ORTIZ DE ROSAS BV (ESQUINA CALLE 25 BIS), Brandsen, Buenos Aires</t>
   </si>
   <si>
@@ -865,6 +1180,12 @@
     <t xml:space="preserve">-58.2159315204996</t>
   </si>
   <si>
+    <t xml:space="preserve">-35.17506237575827</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.21591433317759</t>
+  </si>
+  <si>
     <t xml:space="preserve">BELGRANO MANUEL 130, Brandsen, Buenos Aires</t>
   </si>
   <si>
@@ -874,16 +1195,28 @@
     <t xml:space="preserve">-58.23770947033942</t>
   </si>
   <si>
-    <t xml:space="preserve">RUTA NAC 205 209, Saladillo, Buenos Aires</t>
+    <t xml:space="preserve">-35.162619678201956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.237185248520866</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOS NOGALES (ENTRE LOS LAURELES Y LOS PERALES), Saladillo, Buenos Aires</t>
   </si>
   <si>
     <t xml:space="preserve">Saladillo</t>
   </si>
   <si>
-    <t xml:space="preserve">-35.62728208575118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-59.780078526293245</t>
+    <t xml:space="preserve">-35.6121316631203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-59.791125396257954</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-35.61206400643165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-59.79111326671395</t>
   </si>
   <si>
     <t xml:space="preserve">ELIAS VEDOYA 3632, Lanús, Buenos Aires</t>
@@ -895,6 +1228,12 @@
     <t xml:space="preserve">-58.40640046086712</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.72515120351912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.40598046018701</t>
+  </si>
+  <si>
     <t xml:space="preserve">C COLON 1077, Luján, Buenos Aires</t>
   </si>
   <si>
@@ -907,16 +1246,28 @@
     <t xml:space="preserve">-59.11539102630321</t>
   </si>
   <si>
-    <t xml:space="preserve">AV REPUBLICA ARGENTINA 5200, Pilar, Buenos Aires</t>
+    <t xml:space="preserve">-34.56586802781812</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-59.11560788359534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VICTOR VERGANI 700, Pilar, Buenos Aires</t>
   </si>
   <si>
     <t xml:space="preserve">Pilar</t>
   </si>
   <si>
-    <t xml:space="preserve">-34.4075630070683</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-58.7872211352847</t>
+    <t xml:space="preserve">-34.4592292873655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.9103308497276</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-34.4589819716697</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.910427117872075</t>
   </si>
   <si>
     <t xml:space="preserve">CALLE 791 (ENTRE CALLE 2 Y CALLE 4), General Pueyrredón, Buenos Aires</t>
@@ -931,6 +1282,12 @@
     <t xml:space="preserve">-57.681299048747206</t>
   </si>
   <si>
+    <t xml:space="preserve">-38.199562635644504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.68133639739585</t>
+  </si>
+  <si>
     <t xml:space="preserve">COSME BECCAR 31, San Isidro, Buenos Aires</t>
   </si>
   <si>
@@ -940,6 +1297,12 @@
     <t xml:space="preserve">-58.511873252200935</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.47321453336268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.51179037554271</t>
+  </si>
+  <si>
     <t xml:space="preserve">C 90 - LEANDRO N ALEM 2942, General Pueyrredón, Buenos Aires</t>
   </si>
   <si>
@@ -949,6 +1312,12 @@
     <t xml:space="preserve">-57.530942190256056</t>
   </si>
   <si>
+    <t xml:space="preserve">-38.02148368251992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.530893210210884</t>
+  </si>
+  <si>
     <t xml:space="preserve">MADRID 100, Lomas de Zamora, Buenos Aires</t>
   </si>
   <si>
@@ -958,6 +1327,12 @@
     <t xml:space="preserve">-58.4377153104088</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.76912442087045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.43761790621265</t>
+  </si>
+  <si>
     <t xml:space="preserve">237 PATRICIOS 400, Quilmes, Buenos Aires</t>
   </si>
   <si>
@@ -970,6 +1345,12 @@
     <t xml:space="preserve">-58.2647471240232</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.70998398360919</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.268850248544354</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALLE 122 GRL ROCA 3900, General San Martín, Buenos Aires</t>
   </si>
   <si>
@@ -979,6 +1360,12 @@
     <t xml:space="preserve">-58.5668182782156</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.5562796023699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.56689026895214</t>
+  </si>
+  <si>
     <t xml:space="preserve">RANCHOS 1600, Morón, Buenos Aires</t>
   </si>
   <si>
@@ -988,6 +1375,12 @@
     <t xml:space="preserve">-58.62979422354</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.6455997349856</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.62973653135543</t>
+  </si>
+  <si>
     <t xml:space="preserve">12 ALSINA 100, Quilmes, Buenos Aires</t>
   </si>
   <si>
@@ -997,6 +1390,12 @@
     <t xml:space="preserve">-58.2597158881103</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.722178690123414</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.259720431351454</t>
+  </si>
+  <si>
     <t xml:space="preserve">DR MARIANO MORENO 1500, Vicente López, Buenos Aires</t>
   </si>
   <si>
@@ -1006,6 +1405,12 @@
     <t xml:space="preserve">-58.49747536384576</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.49932521120081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.497820460198746</t>
+  </si>
+  <si>
     <t xml:space="preserve">ITUZAINGO 300, Luján, Buenos Aires</t>
   </si>
   <si>
@@ -1015,6 +1420,12 @@
     <t xml:space="preserve">-59.1193927810945</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.56807191807039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-59.11919648903069</t>
+  </si>
+  <si>
     <t xml:space="preserve">BELGRANO 2100, San Fernando, Buenos Aires</t>
   </si>
   <si>
@@ -1027,6 +1438,12 @@
     <t xml:space="preserve">-58.55062246594373</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.44920465820792</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.550653377393544</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALLE 54 1576, La Plata, Buenos Aires</t>
   </si>
   <si>
@@ -1036,6 +1453,12 @@
     <t xml:space="preserve">-57.967149978159554</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.93505715367856</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.967137789011836</t>
+  </si>
+  <si>
     <t xml:space="preserve">AV GDOR VERGARA 2463, Hurlingham, Buenos Aires</t>
   </si>
   <si>
@@ -1048,6 +1471,12 @@
     <t xml:space="preserve">-58.63451381964711</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.61343379520994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.634454663892036</t>
+  </si>
+  <si>
     <t xml:space="preserve">FELIX FRIAS 2500, Hurlingham, Buenos Aires</t>
   </si>
   <si>
@@ -1057,6 +1486,12 @@
     <t xml:space="preserve">-58.6367470908558</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.6031111633598</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.63743586389262</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALLE 61 LACROZE 5115, General San Martín, Buenos Aires</t>
   </si>
   <si>
@@ -1066,6 +1501,12 @@
     <t xml:space="preserve">-58.55596191804494</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.54631738110748</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.55597406389544</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALLE 79 ARISTOBULO DEL VALLE 4851, General San Martín, Buenos Aires</t>
   </si>
   <si>
@@ -1075,6 +1516,12 @@
     <t xml:space="preserve">-58.55987525954366</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.55421946682352</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.55972256019583</t>
+  </si>
+  <si>
     <t xml:space="preserve">LOS CRISANTEMOS 400, Pilar, Buenos Aires</t>
   </si>
   <si>
@@ -1084,6 +1531,12 @@
     <t xml:space="preserve">-58.78566336301925</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.43606183188628</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.79723578764455</t>
+  </si>
+  <si>
     <t xml:space="preserve">MADARIAGA J GRL 750, Esteban Echeverría, Buenos Aires</t>
   </si>
   <si>
@@ -1093,13 +1546,28 @@
     <t xml:space="preserve">-58.44562683587255</t>
   </si>
   <si>
-    <t xml:space="preserve">GAMARRA SUBTTE IGNACIO 111, Esteban Echeverría, Buenos Aires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-34.8044302289085</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-58.45463307980306</t>
+    <t xml:space="preserve">-34.81107977971013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.44366193134707</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUNTA LARA 266, Mar Chiquita, Buenos Aires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santa Clara del Mar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-37.83751973044875</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.50367230968616</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-37.83750450189813</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.5039031195409</t>
   </si>
   <si>
     <t xml:space="preserve">CAP CLAUDIO N ROSALES 444, Esteban Echeverría, Buenos Aires</t>
@@ -1111,6 +1579,12 @@
     <t xml:space="preserve">-58.442351110602104</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.805471638419604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.4412145755255</t>
+  </si>
+  <si>
     <t xml:space="preserve">C - SANTIAGO DEL ESTERO (ESQUINA C BUENOS AIRES), Tigre, Buenos Aires</t>
   </si>
   <si>
@@ -1120,6 +1594,12 @@
     <t xml:space="preserve">-58.6327389815431</t>
   </si>
   <si>
+    <t xml:space="preserve">-34.45777099174576</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.632727162050436</t>
+  </si>
+  <si>
     <t xml:space="preserve">CHACABUCO 856, Vicente López, Buenos Aires</t>
   </si>
   <si>
@@ -1129,13 +1609,25 @@
     <t xml:space="preserve">-58.48443657736215</t>
   </si>
   <si>
-    <t xml:space="preserve">CALLE 51 749, La Plata, Buenos Aires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-34.97637175988283</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-58.01613167771309</t>
+    <t xml:space="preserve">-34.53211122645095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-58.48497681786831</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALLE 48 633, La Plata, Buenos Aires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-34.91404501791735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.951583759465414</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-34.91404732214143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.952164492712036</t>
   </si>
   <si>
     <t xml:space="preserve">CALLE 23 (ENTRE CALLE 18 Y CALLE 20), La Costa, Buenos Aires</t>
@@ -1150,6 +1642,12 @@
     <t xml:space="preserve">-56.7056045083597</t>
   </si>
   <si>
+    <t xml:space="preserve">-36.48301587068181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-56.705563926173</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALLE 17 700, La Costa, Buenos Aires</t>
   </si>
   <si>
@@ -1159,6 +1657,12 @@
     <t xml:space="preserve">-56.7024547869326</t>
   </si>
   <si>
+    <t xml:space="preserve">-36.48192400197653</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-56.702531204272404</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALLE 531 268, La Plata, Buenos Aires</t>
   </si>
   <si>
@@ -1166,6 +1670,12 @@
   </si>
   <si>
     <t xml:space="preserve">-57.96016976136618</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-34.89096276977386</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-57.96026236017845</t>
   </si>
 </sst>
 </file>
@@ -1275,13 +1785,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F50" activeCellId="0" sqref="F50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53.49"/>
   </cols>
@@ -1305,87 +1815,84 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1542,1261 +2049,1771 @@
       <c r="D13" s="0" t="s">
         <v>71</v>
       </c>
+      <c r="E13" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>69</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>111</v>
+        <v>121</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>114</v>
+        <v>126</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>117</v>
+        <v>131</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>121</v>
+        <v>137</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>127</v>
+        <v>147</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>130</v>
+        <v>152</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>134</v>
+        <v>158</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>137</v>
+        <v>163</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>140</v>
+        <v>168</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>143</v>
+        <v>173</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>146</v>
+        <v>178</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>147</v>
+        <v>181</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>149</v>
+        <v>183</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>152</v>
+        <v>188</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>153</v>
+        <v>189</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>155</v>
+        <v>193</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>156</v>
+        <v>194</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>157</v>
+        <v>197</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>158</v>
+        <v>198</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>160</v>
+        <v>200</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>161</v>
+        <v>203</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>158</v>
+        <v>198</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>162</v>
+        <v>204</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>163</v>
+        <v>205</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>164</v>
+        <v>208</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>165</v>
+        <v>209</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>166</v>
+        <v>210</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>167</v>
+        <v>211</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>168</v>
+        <v>214</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>165</v>
+        <v>209</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>169</v>
+        <v>215</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>170</v>
+        <v>216</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>171</v>
+        <v>219</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>172</v>
+        <v>220</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>173</v>
+        <v>221</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>174</v>
+        <v>222</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>175</v>
+        <v>225</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>177</v>
+        <v>227</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>178</v>
+        <v>228</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>179</v>
+        <v>231</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>180</v>
+        <v>232</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>181</v>
+        <v>233</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>182</v>
+        <v>234</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>183</v>
+        <v>237</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>184</v>
+        <v>238</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>185</v>
+        <v>239</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>186</v>
+        <v>242</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>187</v>
+        <v>243</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>188</v>
+        <v>244</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>189</v>
+        <v>245</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>190</v>
+        <v>248</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>191</v>
+        <v>249</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>192</v>
+        <v>250</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>193</v>
+        <v>251</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>194</v>
+        <v>254</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>191</v>
+        <v>249</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>195</v>
+        <v>255</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>196</v>
+        <v>256</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>197</v>
+        <v>259</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>198</v>
+        <v>260</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>199</v>
+        <v>261</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>200</v>
+        <v>262</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>201</v>
+        <v>265</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>202</v>
+        <v>266</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>203</v>
+        <v>267</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>204</v>
+        <v>268</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>205</v>
+        <v>271</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>206</v>
+        <v>272</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>207</v>
+        <v>273</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>208</v>
+        <v>274</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>209</v>
+        <v>277</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>210</v>
+        <v>266</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>211</v>
+        <v>278</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>212</v>
+        <v>279</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>213</v>
+        <v>282</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>206</v>
+        <v>272</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>214</v>
+        <v>283</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>215</v>
+        <v>284</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>216</v>
+        <v>287</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>217</v>
+        <v>288</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>218</v>
+        <v>289</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>219</v>
+        <v>290</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>220</v>
+        <v>293</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>217</v>
+        <v>288</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>221</v>
+        <v>294</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>222</v>
+        <v>295</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>223</v>
+        <v>298</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>217</v>
+        <v>288</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>224</v>
+        <v>299</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>225</v>
+        <v>300</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>226</v>
+        <v>303</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>227</v>
+        <v>304</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>228</v>
+        <v>305</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>229</v>
+        <v>306</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>230</v>
+        <v>309</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>231</v>
+        <v>310</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>232</v>
+        <v>311</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>233</v>
+        <v>312</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>234</v>
+        <v>315</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>231</v>
+        <v>310</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>235</v>
+        <v>316</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>236</v>
+        <v>317</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>237</v>
+        <v>320</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>238</v>
+        <v>321</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>239</v>
+        <v>322</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>240</v>
+        <v>323</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>241</v>
+        <v>326</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>242</v>
+        <v>327</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>243</v>
+        <v>328</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>244</v>
+        <v>329</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>245</v>
+        <v>332</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>242</v>
+        <v>327</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>246</v>
+        <v>333</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>247</v>
+        <v>334</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>248</v>
+        <v>337</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>249</v>
+        <v>338</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>250</v>
+        <v>339</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>251</v>
+        <v>340</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>252</v>
+        <v>343</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>253</v>
+        <v>344</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>254</v>
+        <v>345</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>255</v>
+        <v>346</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>256</v>
+        <v>349</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>257</v>
+        <v>350</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>258</v>
+        <v>351</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>259</v>
+        <v>352</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>260</v>
+        <v>355</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>242</v>
+        <v>327</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>261</v>
+        <v>356</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>262</v>
+        <v>357</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>263</v>
+        <v>360</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>264</v>
+        <v>361</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>265</v>
+        <v>362</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>266</v>
+        <v>363</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>267</v>
+        <v>366</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>264</v>
+        <v>361</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>268</v>
+        <v>367</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>269</v>
+        <v>368</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>270</v>
+        <v>371</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>242</v>
+        <v>327</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>271</v>
+        <v>372</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>272</v>
+        <v>373</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>273</v>
+        <v>376</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>274</v>
+        <v>377</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>275</v>
+        <v>378</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>276</v>
+        <v>379</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>277</v>
+        <v>382</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>278</v>
+        <v>383</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>279</v>
+        <v>384</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>280</v>
+        <v>385</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>281</v>
+        <v>388</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>278</v>
+        <v>383</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>282</v>
+        <v>389</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>283</v>
+        <v>390</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>284</v>
+        <v>393</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>285</v>
+        <v>394</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>286</v>
+        <v>395</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>287</v>
+        <v>396</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>288</v>
+        <v>399</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>30</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>289</v>
+        <v>400</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>290</v>
+        <v>401</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>291</v>
+        <v>404</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>292</v>
+        <v>405</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>293</v>
+        <v>406</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>294</v>
+        <v>407</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>295</v>
+        <v>410</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>296</v>
+        <v>411</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>297</v>
+        <v>412</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>298</v>
+        <v>413</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>299</v>
+        <v>416</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>300</v>
+        <v>417</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>301</v>
+        <v>418</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>302</v>
+        <v>419</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>303</v>
+        <v>422</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>304</v>
+        <v>423</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>305</v>
+        <v>424</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>306</v>
+        <v>427</v>
       </c>
       <c r="B78" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>307</v>
+        <v>428</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>308</v>
+        <v>429</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>309</v>
+        <v>432</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>249</v>
+        <v>338</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>310</v>
+        <v>433</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>311</v>
+        <v>434</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>312</v>
+        <v>437</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>313</v>
+        <v>438</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>314</v>
+        <v>439</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>315</v>
+        <v>440</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>316</v>
+        <v>443</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>238</v>
+        <v>321</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>317</v>
+        <v>444</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>318</v>
+        <v>445</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>319</v>
+        <v>448</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>41</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>320</v>
+        <v>449</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>321</v>
+        <v>450</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>322</v>
+        <v>453</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>313</v>
+        <v>438</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>323</v>
+        <v>454</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>324</v>
+        <v>455</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>325</v>
+        <v>458</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>253</v>
+        <v>344</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>326</v>
+        <v>459</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>327</v>
+        <v>460</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>328</v>
+        <v>463</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>292</v>
+        <v>405</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>329</v>
+        <v>464</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>330</v>
+        <v>465</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>331</v>
+        <v>468</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>332</v>
+        <v>469</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>333</v>
+        <v>470</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>334</v>
+        <v>471</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>335</v>
+        <v>474</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>336</v>
+        <v>475</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>337</v>
+        <v>476</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>338</v>
+        <v>479</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>339</v>
+        <v>480</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>340</v>
+        <v>481</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>341</v>
+        <v>482</v>
+      </c>
+      <c r="E88" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>342</v>
+        <v>485</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>339</v>
+        <v>480</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>343</v>
+        <v>486</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>344</v>
+        <v>487</v>
+      </c>
+      <c r="E89" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>345</v>
+        <v>490</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>238</v>
+        <v>321</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>346</v>
+        <v>491</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>347</v>
+        <v>492</v>
+      </c>
+      <c r="E90" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>348</v>
+        <v>495</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>238</v>
+        <v>321</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>349</v>
+        <v>496</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>350</v>
+        <v>497</v>
+      </c>
+      <c r="E91" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>351</v>
+        <v>500</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>296</v>
+        <v>411</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>352</v>
+        <v>501</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>353</v>
+        <v>502</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>354</v>
+        <v>505</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>355</v>
+        <v>506</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>356</v>
+        <v>507</v>
+      </c>
+      <c r="E93" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>357</v>
+        <v>510</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>151</v>
+        <v>511</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>358</v>
+        <v>512</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>359</v>
+        <v>513</v>
+      </c>
+      <c r="E94" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>360</v>
+        <v>516</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>361</v>
+        <v>517</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>362</v>
+        <v>518</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>363</v>
+        <v>521</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>364</v>
+        <v>522</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>365</v>
+        <v>523</v>
+      </c>
+      <c r="E96" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>366</v>
+        <v>526</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>253</v>
+        <v>344</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>367</v>
+        <v>527</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>368</v>
+        <v>528</v>
+      </c>
+      <c r="E97" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>369</v>
+        <v>531</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>370</v>
+        <v>532</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>371</v>
+        <v>533</v>
+      </c>
+      <c r="E98" s="0" t="s">
+        <v>534</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>372</v>
+        <v>536</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>373</v>
+        <v>537</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>374</v>
+        <v>538</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>375</v>
+        <v>539</v>
+      </c>
+      <c r="E99" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>376</v>
+        <v>542</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>373</v>
+        <v>537</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>377</v>
+        <v>543</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>378</v>
+        <v>544</v>
+      </c>
+      <c r="E100" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>379</v>
+        <v>547</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>380</v>
+        <v>548</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>381</v>
+        <v>549</v>
+      </c>
+      <c r="E101" s="0" t="s">
+        <v>550</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>